<commit_message>
Feb 22 2019 - FIREVAT operational. Implemented Variant annotation, strand bias analysis, mutational signature analysis optimization
</commit_message>
<xml_diff>
--- a/inst/docs/Report_Components.xlsx
+++ b/inst/docs/Report_Components.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t xml:space="preserve">MODE</t>
   </si>
@@ -124,10 +124,16 @@
     <t xml:space="preserve">OPTIONAL_4</t>
   </si>
   <si>
-    <t xml:space="preserve">Annotation Table</t>
+    <t xml:space="preserve">Refined Annotation Table</t>
   </si>
   <si>
     <t xml:space="preserve">optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTIONAL_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artifact Annotation Table</t>
   </si>
 </sst>
 </file>
@@ -142,6 +148,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -164,6 +171,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -233,16 +241,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -339,10 +343,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,60 +366,60 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -423,64 +427,64 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="0" t="s">
@@ -488,19 +492,19 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -508,19 +512,19 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="0" t="s">
@@ -528,19 +532,19 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="C12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="0" t="s">
@@ -548,19 +552,19 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="0" t="s">
@@ -568,19 +572,19 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="0" t="s">
@@ -588,19 +592,19 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -608,22 +612,42 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>